<commit_message>
update paths to cloud
</commit_message>
<xml_diff>
--- a/models/interpretations/entities_analysis/missed_annotation.xlsx
+++ b/models/interpretations/entities_analysis/missed_annotation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prl222/OneDrive - The Open University/Projects/hate-speech-identities/models/interpretations/entities_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B67253B-3D72-514D-8884-FEB6CB3F78A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B9E196-4181-AC44-B681-39446C5D9CDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="missed_annotation" sheetId="1" r:id="rId1"/>
@@ -28,21 +28,9 @@
     <t>comment_id</t>
   </si>
   <si>
-    <t>logits_y_trues</t>
-  </si>
-  <si>
     <t>error_sample_logits</t>
   </si>
   <si>
-    <t>Error_UniCategories</t>
-  </si>
-  <si>
-    <t>logits_pos_matches</t>
-  </si>
-  <si>
-    <t>logits_neg_matches</t>
-  </si>
-  <si>
     <t>annotation</t>
   </si>
   <si>
@@ -209,12 +197,24 @@
   </si>
   <si>
     <t>19162195_gab</t>
+  </si>
+  <si>
+    <t>HybridLR$_{h}$_y_trues</t>
+  </si>
+  <si>
+    <t>HybridLR$_{h}$_pos_matches</t>
+  </si>
+  <si>
+    <t>HybridLR$_{h}$_neg_matches</t>
+  </si>
+  <si>
+    <t>Error_Categories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1048,10 +1048,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1063,33 +1065,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>13326</v>
@@ -1101,27 +1103,27 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>8096</v>
@@ -1133,27 +1135,27 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>532</v>
@@ -1165,24 +1167,24 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>23370</v>
@@ -1194,24 +1196,24 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>11249</v>
@@ -1223,27 +1225,27 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>7737</v>
@@ -1255,24 +1257,24 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
         <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>20614</v>
@@ -1284,24 +1286,24 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
         <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>25306</v>
@@ -1313,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>18921</v>
@@ -1342,24 +1344,24 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>15141</v>
@@ -1371,27 +1373,27 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>13858</v>
@@ -1403,24 +1405,24 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>15625</v>
@@ -1432,27 +1434,27 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
         <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1461,59 +1463,59 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
         <v>35</v>
       </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1522,30 +1524,30 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
         <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1554,30 +1556,30 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1586,30 +1588,30 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1618,30 +1620,30 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1650,27 +1652,27 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
         <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1679,27 +1681,27 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I21">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1708,30 +1710,30 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
         <v>11</v>
-      </c>
-      <c r="F22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1740,27 +1742,27 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1769,19 +1771,19 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>